<commit_message>
Swapped members in batch1, use pre for code blocks in maven, rest api & added scope table for maven
</commit_message>
<xml_diff>
--- a/Teams Progress/batch1-2025-teams.xlsx
+++ b/Teams Progress/batch1-2025-teams.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Professional Documents\Training-Teaching\bv-raju\training-materials\Teams Progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{550FFA3B-D424-499A-97F5-A0CB8AED7DEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23293B1A-CF9D-4F47-B6E8-065C2A891661}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Student-Teams" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Student-Teams'!$A$1:$E$148</definedName>
@@ -24,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="767" uniqueCount="467">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="741" uniqueCount="465">
   <si>
     <t>Student ID</t>
   </si>
@@ -239,15 +238,6 @@
     <t>23B01A0586</t>
   </si>
   <si>
-    <t>24</t>
-  </si>
-  <si>
-    <t>YARLAGADDA JANAKI</t>
-  </si>
-  <si>
-    <t>23B01A42D1</t>
-  </si>
-  <si>
     <t>Team_2</t>
   </si>
   <si>
@@ -305,15 +295,6 @@
     <t>23B01A1232</t>
   </si>
   <si>
-    <t>25</t>
-  </si>
-  <si>
-    <t>YARRAVULA ROOSHITHA</t>
-  </si>
-  <si>
-    <t>23B01A42D2</t>
-  </si>
-  <si>
     <t>100</t>
   </si>
   <si>
@@ -1238,15 +1219,6 @@
     <t>23B01A0548</t>
   </si>
   <si>
-    <t>23</t>
-  </si>
-  <si>
-    <t>VELUPURI GANGA GOWRI</t>
-  </si>
-  <si>
-    <t>23B01A42C6</t>
-  </si>
-  <si>
     <t>120</t>
   </si>
   <si>
@@ -1425,6 +1397,27 @@
   </si>
   <si>
     <t>Git Team Creation</t>
+  </si>
+  <si>
+    <t>MUNGANDA DIVIJA</t>
+  </si>
+  <si>
+    <t>??</t>
+  </si>
+  <si>
+    <t>23B01A4280</t>
+  </si>
+  <si>
+    <t>23B01A4298</t>
+  </si>
+  <si>
+    <t>PERURI BHAVYA RATNA</t>
+  </si>
+  <si>
+    <t>VASAMSETTI VIJAYA KRISHNA TAPASWI</t>
+  </si>
+  <si>
+    <t>23B01A42C4</t>
   </si>
 </sst>
 </file>
@@ -1834,7 +1827,7 @@
   <dimension ref="A1:F148"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H112" sqref="H112"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1864,7 +1857,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>466</v>
+        <v>457</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -2210,2335 +2203,2171 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>71</v>
+        <v>459</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>72</v>
+        <v>458</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>73</v>
+        <v>460</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>74</v>
+        <v>379</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>24</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>93</v>
+        <v>459</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>94</v>
+        <v>462</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>95</v>
+        <v>461</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>17</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="D58" s="3" t="s">
         <v>17</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="D65" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="D66" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+        <v>193</v>
+      </c>
+      <c r="F66" s="5"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="D70" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E73" s="2" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A74" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="C74" s="2" t="s">
         <v>230</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A74" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>236</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" s="3" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="D75" s="3" t="s">
         <v>24</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="D76" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="D77" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="D79" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="D80" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="D81" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="D82" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="D83" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D85" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="D86" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" s="3" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="D87" s="3" t="s">
         <v>24</v>
       </c>
       <c r="E87" s="3" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="D88" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="D89" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="D90" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="D91" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="D92" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="D93" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="D94" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="D95" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="D96" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="B97" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="C97" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="D97" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E97" s="3" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A98" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="D98" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E98" s="2" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A99" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="B97" s="3" t="s">
+      <c r="B99" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="C97" s="3" t="s">
+      <c r="C99" s="2" t="s">
         <v>307</v>
-      </c>
-      <c r="D97" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E97" s="3" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A98" s="2" t="s">
-        <v>308</v>
-      </c>
-      <c r="B98" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="C98" s="2" t="s">
-        <v>310</v>
-      </c>
-      <c r="D98" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E98" s="2" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A99" s="2" t="s">
-        <v>311</v>
-      </c>
-      <c r="B99" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="C99" s="2" t="s">
-        <v>313</v>
       </c>
       <c r="D99" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="D100" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E100" s="2" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A101" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="D101" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E101" s="2" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A102" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="B100" s="2" t="s">
+      <c r="B102" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="C100" s="2" t="s">
+      <c r="C102" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="D100" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E100" s="2" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A101" s="2" t="s">
+      <c r="D102" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E102" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="B101" s="2" t="s">
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A103" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="C101" s="2" t="s">
+      <c r="B103" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="D101" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E101" s="2" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A102" s="2" t="s">
+      <c r="C103" s="2" t="s">
         <v>320</v>
-      </c>
-      <c r="B102" s="2" t="s">
-        <v>321</v>
-      </c>
-      <c r="C102" s="2" t="s">
-        <v>322</v>
-      </c>
-      <c r="D102" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E102" s="2" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A103" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="B103" s="2" t="s">
-        <v>325</v>
-      </c>
-      <c r="C103" s="2" t="s">
-        <v>326</v>
       </c>
       <c r="D103" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E103" s="2" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A104" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="C104" s="2" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A104" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="B104" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="C104" s="2" t="s">
-        <v>329</v>
-      </c>
       <c r="D104" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E104" s="2" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="D105" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E105" s="2" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="E106" s="2" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A107" s="2" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="D107" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E107" s="2" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A108" s="2" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="D108" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E108" s="2" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="D109" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E109" s="2" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A110" s="3" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="C110" s="3" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="D110" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E110" s="3" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+        <v>317</v>
+      </c>
+      <c r="F110" s="5"/>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A111" s="2" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D111" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E111" s="2" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A112" s="3" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="C112" s="3" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D112" s="3" t="s">
         <v>17</v>
       </c>
       <c r="E112" s="3" t="s">
-        <v>354</v>
-      </c>
+        <v>348</v>
+      </c>
+      <c r="F112" s="5"/>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="D113" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E113" s="2" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" s="2" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="D114" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E114" s="2" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="D115" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E115" s="2" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
       <c r="D116" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E116" s="2" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117" s="2" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="D117" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E117" s="2" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" s="2" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="D118" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E118" s="2" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" s="2" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
       <c r="D119" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E119" s="2" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120" s="2" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="D120" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E120" s="2" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121" s="2" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>380</v>
+        <v>374</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="E121" s="2" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" s="2" t="s">
-        <v>382</v>
+        <v>376</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>383</v>
+        <v>377</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>384</v>
+        <v>378</v>
       </c>
       <c r="D122" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E122" s="2" t="s">
-        <v>385</v>
+        <v>379</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" s="2" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
       <c r="D123" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E123" s="2" t="s">
-        <v>385</v>
+        <v>379</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" s="2" t="s">
-        <v>389</v>
+        <v>383</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>390</v>
+        <v>384</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
       <c r="D124" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E124" s="2" t="s">
-        <v>385</v>
+        <v>379</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125" s="2" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>393</v>
+        <v>387</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>394</v>
+        <v>388</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="E125" s="2" t="s">
-        <v>385</v>
+        <v>379</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126" s="2" t="s">
-        <v>395</v>
+        <v>389</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>397</v>
+        <v>391</v>
       </c>
       <c r="D126" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E126" s="2" t="s">
-        <v>385</v>
+        <v>379</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127" s="2" t="s">
-        <v>398</v>
+        <v>392</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>399</v>
+        <v>393</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>400</v>
+        <v>394</v>
       </c>
       <c r="D127" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E127" s="2" t="s">
-        <v>385</v>
+        <v>379</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128" s="2" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
       <c r="D128" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E128" s="2" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A129" s="2" t="s">
-        <v>404</v>
+        <v>459</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>405</v>
+        <v>463</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>406</v>
+        <v>464</v>
       </c>
       <c r="D129" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E129" s="2" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A130" s="3" t="s">
-        <v>407</v>
+        <v>398</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>408</v>
+        <v>399</v>
       </c>
       <c r="C130" s="3" t="s">
-        <v>409</v>
+        <v>400</v>
       </c>
       <c r="D130" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E130" s="3" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
+        <v>379</v>
+      </c>
+      <c r="F130" s="5"/>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A131" s="2" t="s">
-        <v>410</v>
+        <v>401</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>411</v>
+        <v>402</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>412</v>
+        <v>403</v>
       </c>
       <c r="D131" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E131" s="2" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A132" s="2" t="s">
-        <v>413</v>
+        <v>404</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>414</v>
+        <v>405</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>415</v>
+        <v>406</v>
       </c>
       <c r="D132" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E132" s="2" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A133" s="3" t="s">
-        <v>417</v>
+        <v>408</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>418</v>
+        <v>409</v>
       </c>
       <c r="C133" s="3" t="s">
-        <v>419</v>
+        <v>410</v>
       </c>
       <c r="D133" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E133" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="F133" s="5"/>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A134" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="B134" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="C134" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="D134" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E134" s="2" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A135" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="B135" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="C135" s="2" t="s">
         <v>416</v>
-      </c>
-    </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A134" s="2" t="s">
-        <v>420</v>
-      </c>
-      <c r="B134" s="2" t="s">
-        <v>421</v>
-      </c>
-      <c r="C134" s="2" t="s">
-        <v>422</v>
-      </c>
-      <c r="D134" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E134" s="2" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A135" s="2" t="s">
-        <v>423</v>
-      </c>
-      <c r="B135" s="2" t="s">
-        <v>424</v>
-      </c>
-      <c r="C135" s="2" t="s">
-        <v>425</v>
       </c>
       <c r="D135" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E135" s="2" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A136" s="2" t="s">
-        <v>426</v>
+        <v>417</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>427</v>
+        <v>418</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>428</v>
+        <v>419</v>
       </c>
       <c r="D136" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E136" s="2" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A137" s="2" t="s">
-        <v>429</v>
+        <v>420</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>430</v>
+        <v>421</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>431</v>
+        <v>422</v>
       </c>
       <c r="D137" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E137" s="2" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A138" s="2" t="s">
-        <v>432</v>
+        <v>423</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>433</v>
+        <v>424</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>434</v>
+        <v>425</v>
       </c>
       <c r="D138" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E138" s="2" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A139" s="2" t="s">
-        <v>435</v>
+        <v>426</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>436</v>
+        <v>427</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>437</v>
+        <v>428</v>
       </c>
       <c r="D139" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E139" s="2" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A140" s="2" t="s">
-        <v>438</v>
+        <v>429</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>439</v>
+        <v>430</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>440</v>
+        <v>431</v>
       </c>
       <c r="D140" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E140" s="2" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A141" s="2" t="s">
-        <v>441</v>
+        <v>432</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>442</v>
+        <v>433</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>443</v>
+        <v>434</v>
       </c>
       <c r="D141" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E141" s="2" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A142" s="2" t="s">
-        <v>444</v>
+        <v>435</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>445</v>
+        <v>436</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>446</v>
+        <v>437</v>
       </c>
       <c r="D142" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E142" s="2" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A143" s="2" t="s">
-        <v>448</v>
+        <v>439</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>449</v>
+        <v>440</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>450</v>
+        <v>441</v>
       </c>
       <c r="D143" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E143" s="2" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A144" s="2" t="s">
-        <v>451</v>
+        <v>442</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>452</v>
+        <v>443</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>453</v>
+        <v>444</v>
       </c>
       <c r="D144" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E144" s="2" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A145" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="B145" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="C145" s="2" t="s">
         <v>447</v>
       </c>
-    </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A145" s="2" t="s">
+      <c r="D145" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E145" s="2" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A146" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="B146" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="C146" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="D146" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E146" s="2" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A147" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="B147" s="2" t="s">
+        <v>452</v>
+      </c>
+      <c r="C147" s="2" t="s">
+        <v>453</v>
+      </c>
+      <c r="D147" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E147" s="2" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A148" s="3" t="s">
         <v>454</v>
       </c>
-      <c r="B145" s="2" t="s">
+      <c r="B148" s="3" t="s">
         <v>455</v>
       </c>
-      <c r="C145" s="2" t="s">
+      <c r="C148" s="3" t="s">
         <v>456</v>
-      </c>
-      <c r="D145" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E145" s="2" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A146" s="2" t="s">
-        <v>457</v>
-      </c>
-      <c r="B146" s="2" t="s">
-        <v>458</v>
-      </c>
-      <c r="C146" s="2" t="s">
-        <v>459</v>
-      </c>
-      <c r="D146" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E146" s="2" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A147" s="2" t="s">
-        <v>460</v>
-      </c>
-      <c r="B147" s="2" t="s">
-        <v>461</v>
-      </c>
-      <c r="C147" s="2" t="s">
-        <v>462</v>
-      </c>
-      <c r="D147" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E147" s="2" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A148" s="3" t="s">
-        <v>463</v>
-      </c>
-      <c r="B148" s="3" t="s">
-        <v>464</v>
-      </c>
-      <c r="C148" s="3" t="s">
-        <v>465</v>
       </c>
       <c r="D148" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E148" s="3" t="s">
-        <v>447</v>
-      </c>
+        <v>438</v>
+      </c>
+      <c r="F148" s="5"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:E148" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74A400A7-C5E1-47EE-945C-E66DF8A23769}">
-  <dimension ref="A1:E15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2">
-        <f>COUNTIF($B$1:$B$15,D2)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>323</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3">
-        <f t="shared" ref="E3:E6" si="0">COUNTIF($B$1:$B$15,D3)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>354</v>
-      </c>
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>385</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>416</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" t="s">
-        <v>105</v>
-      </c>
-      <c r="E6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>14</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>2</v>
-      </c>
-      <c r="B8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>3</v>
-      </c>
-      <c r="B9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>4</v>
-      </c>
-      <c r="B10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>5</v>
-      </c>
-      <c r="B11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>6</v>
-      </c>
-      <c r="B12" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>7</v>
-      </c>
-      <c r="B13" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>8</v>
-      </c>
-      <c r="B14" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>9</v>
-      </c>
-      <c r="B15" t="s">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Added lambda and other material
</commit_message>
<xml_diff>
--- a/Teams Progress/batch1-2025-teams.xlsx
+++ b/Teams Progress/batch1-2025-teams.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Professional Documents\Training-Teaching\bv-raju\training-materials\Teams Progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1ABB15F-9A79-4238-A0F0-E897941B9F8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{775754EC-822C-4695-95DD-3824CC6DEC25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1844,7 +1844,7 @@
   <dimension ref="A1:F149"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F75" sqref="F75"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3140,6 +3140,7 @@
       <c r="E75" s="3" t="s">
         <v>224</v>
       </c>
+      <c r="F75" s="5"/>
     </row>
     <row r="76" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">

</xml_diff>